<commit_message>
Enable manage_structure templates page (DB-only, no hardcoded contents)
</commit_message>
<xml_diff>
--- a/public/CRF_Form_Template.xlsx
+++ b/public/CRF_Form_Template.xlsx
@@ -74,7 +74,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -82,9 +82,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -453,7 +454,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -462,8 +463,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="32" customWidth="1" min="1" max="1"/>
-    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="34" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -485,258 +486,363 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr"/>
-      <c r="B2" s="2" t="inlineStr"/>
-      <c r="C2" s="2" t="inlineStr"/>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Demographics</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>DM</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr"/>
-      <c r="B3" s="2" t="inlineStr"/>
-      <c r="C3" s="2" t="inlineStr"/>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Inclusion/Exclusion Criteria</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>IE</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>FALSE</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr"/>
-      <c r="B4" s="2" t="inlineStr"/>
-      <c r="C4" s="2" t="inlineStr"/>
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Medical History</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>MH</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr"/>
-      <c r="B5" s="2" t="inlineStr"/>
-      <c r="C5" s="2" t="inlineStr"/>
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Concomitant Medications</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>CM</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr"/>
-      <c r="B6" s="2" t="inlineStr"/>
-      <c r="C6" s="2" t="inlineStr"/>
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Adverse Events</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>AE</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr"/>
-      <c r="B7" s="2" t="inlineStr"/>
-      <c r="C7" s="2" t="inlineStr"/>
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Serious Adverse Events</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>AE</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr"/>
-      <c r="B8" s="2" t="inlineStr"/>
-      <c r="C8" s="2" t="inlineStr"/>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Vital Signs</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>VS</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="inlineStr"/>
-      <c r="B9" s="2" t="inlineStr"/>
-      <c r="C9" s="2" t="inlineStr"/>
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Physical Examination</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="inlineStr"/>
-      <c r="B10" s="2" t="inlineStr"/>
-      <c r="C10" s="2" t="inlineStr"/>
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Clinical Laboratory Tests</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>LB</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr"/>
-      <c r="B11" s="2" t="inlineStr"/>
-      <c r="C11" s="2" t="inlineStr"/>
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Electrocardiogram</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>EG</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="inlineStr"/>
-      <c r="B12" s="2" t="inlineStr"/>
-      <c r="C12" s="2" t="inlineStr"/>
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>Exposure / IP Administration</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="inlineStr"/>
-      <c r="B13" s="2" t="inlineStr"/>
-      <c r="C13" s="2" t="inlineStr"/>
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Drug Accountability</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>DA</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="inlineStr"/>
-      <c r="B14" s="2" t="inlineStr"/>
-      <c r="C14" s="2" t="inlineStr"/>
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Protocol Deviations</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>DV</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="inlineStr"/>
-      <c r="B15" s="2" t="inlineStr"/>
-      <c r="C15" s="2" t="inlineStr"/>
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>Disposition / Subject Status</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>DS</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr"/>
-      <c r="B16" s="2" t="inlineStr"/>
-      <c r="C16" s="2" t="inlineStr"/>
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>Subject Visits</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>SV</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="inlineStr"/>
       <c r="B17" s="2" t="inlineStr"/>
-      <c r="C17" s="2" t="inlineStr"/>
+      <c r="C17" s="3" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="inlineStr"/>
       <c r="B18" s="2" t="inlineStr"/>
-      <c r="C18" s="2" t="inlineStr"/>
+      <c r="C18" s="3" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr"/>
       <c r="B19" s="2" t="inlineStr"/>
-      <c r="C19" s="2" t="inlineStr"/>
+      <c r="C19" s="3" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr"/>
       <c r="B20" s="2" t="inlineStr"/>
-      <c r="C20" s="2" t="inlineStr"/>
+      <c r="C20" s="3" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr"/>
       <c r="B21" s="2" t="inlineStr"/>
-      <c r="C21" s="2" t="inlineStr"/>
+      <c r="C21" s="3" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr"/>
       <c r="B22" s="2" t="inlineStr"/>
-      <c r="C22" s="2" t="inlineStr"/>
+      <c r="C22" s="3" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="inlineStr"/>
       <c r="B23" s="2" t="inlineStr"/>
-      <c r="C23" s="2" t="inlineStr"/>
+      <c r="C23" s="3" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr"/>
       <c r="B24" s="2" t="inlineStr"/>
-      <c r="C24" s="2" t="inlineStr"/>
+      <c r="C24" s="3" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr"/>
       <c r="B25" s="2" t="inlineStr"/>
-      <c r="C25" s="2" t="inlineStr"/>
+      <c r="C25" s="3" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr"/>
       <c r="B26" s="2" t="inlineStr"/>
-      <c r="C26" s="2" t="inlineStr"/>
+      <c r="C26" s="3" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr"/>
       <c r="B27" s="2" t="inlineStr"/>
-      <c r="C27" s="2" t="inlineStr"/>
+      <c r="C27" s="3" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr"/>
       <c r="B28" s="2" t="inlineStr"/>
-      <c r="C28" s="2" t="inlineStr"/>
+      <c r="C28" s="3" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr"/>
       <c r="B29" s="2" t="inlineStr"/>
-      <c r="C29" s="2" t="inlineStr"/>
+      <c r="C29" s="3" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr"/>
       <c r="B30" s="2" t="inlineStr"/>
-      <c r="C30" s="2" t="inlineStr"/>
+      <c r="C30" s="3" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="inlineStr"/>
       <c r="B31" s="2" t="inlineStr"/>
-      <c r="C31" s="2" t="inlineStr"/>
+      <c r="C31" s="3" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr"/>
       <c r="B32" s="2" t="inlineStr"/>
-      <c r="C32" s="2" t="inlineStr"/>
+      <c r="C32" s="3" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr"/>
       <c r="B33" s="2" t="inlineStr"/>
-      <c r="C33" s="2" t="inlineStr"/>
+      <c r="C33" s="3" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr"/>
       <c r="B34" s="2" t="inlineStr"/>
-      <c r="C34" s="2" t="inlineStr"/>
+      <c r="C34" s="3" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr"/>
       <c r="B35" s="2" t="inlineStr"/>
-      <c r="C35" s="2" t="inlineStr"/>
+      <c r="C35" s="3" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr"/>
       <c r="B36" s="2" t="inlineStr"/>
-      <c r="C36" s="2" t="inlineStr"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="2" t="inlineStr"/>
-      <c r="B37" s="2" t="inlineStr"/>
-      <c r="C37" s="2" t="inlineStr"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="inlineStr"/>
-      <c r="B38" s="2" t="inlineStr"/>
-      <c r="C38" s="2" t="inlineStr"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="2" t="inlineStr"/>
-      <c r="B39" s="2" t="inlineStr"/>
-      <c r="C39" s="2" t="inlineStr"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="2" t="inlineStr"/>
-      <c r="B40" s="2" t="inlineStr"/>
-      <c r="C40" s="2" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="2" t="inlineStr"/>
-      <c r="B41" s="2" t="inlineStr"/>
-      <c r="C41" s="2" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="2" t="inlineStr"/>
-      <c r="B42" s="2" t="inlineStr"/>
-      <c r="C42" s="2" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="inlineStr"/>
-      <c r="B43" s="2" t="inlineStr"/>
-      <c r="C43" s="2" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="inlineStr"/>
-      <c r="B44" s="2" t="inlineStr"/>
-      <c r="C44" s="2" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="inlineStr"/>
-      <c r="B45" s="2" t="inlineStr"/>
-      <c r="C45" s="2" t="inlineStr"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="inlineStr"/>
-      <c r="B46" s="2" t="inlineStr"/>
-      <c r="C46" s="2" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="2" t="inlineStr"/>
-      <c r="B47" s="2" t="inlineStr"/>
-      <c r="C47" s="2" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="2" t="inlineStr"/>
-      <c r="B48" s="2" t="inlineStr"/>
-      <c r="C48" s="2" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="2" t="inlineStr"/>
-      <c r="B49" s="2" t="inlineStr"/>
-      <c r="C49" s="2" t="inlineStr"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="2" t="inlineStr"/>
-      <c r="B50" s="2" t="inlineStr"/>
-      <c r="C50" s="2" t="inlineStr"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="2" t="inlineStr"/>
-      <c r="B51" s="2" t="inlineStr"/>
-      <c r="C51" s="2" t="inlineStr"/>
+      <c r="C36" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="C2:C51" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="C2:C36" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -750,7 +856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -758,79 +864,82 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="90" customWidth="1" min="1" max="1"/>
+    <col width="110" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>사용 방법</t>
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>샘플 CRF Form 목록 (SDTM Form Code 사용)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>1) 'Template' 시트의 빈칸을 채운 뒤, 그대로 업로드하세요.</t>
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>- 본 파일은 CRF Form Builder 업로드용 샘플입니다.</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
-        <is>
-          <t>2) 헤더(첫 줄)는 반드시 아래 3개를 그대로 유지해야 합니다: Form Name / Form Code / Repeat</t>
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>- 헤더(첫 줄): Form Name / Form Code / Repeat 를 변경하지 마세요.</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>3) Repeat 값은 TRUE/FALSE 를 권장합니다. (인식 예: TRUE/FALSE, Y/N, 1/0)</t>
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>- Repeat: TRUE/FALSE 권장 (Y/N, 1/0도 시스템에서 인식 가능).</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>4) 완전히 빈 행은 업로드 시 자동으로 무시됩니다.</t>
-        </is>
-      </c>
+      <c r="A5" s="5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>5) 업로드 시 기존 데이터는 '덮어쓰기' 됩니다(현재 구현 기준).</t>
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>코드 참고(주요 SDTM 도메인)</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr"/>
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>DM: Demographics, IE: Inclusion/Exclusion, MH: Medical History, CM: Concomitant Medications, AE: Adverse Events</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>예시</t>
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>VS: Vital Signs, PE: Physical Exam, LB: Labs, EG: ECG, EX: Exposure, DA: Drug Accountability, DV: Protocol Deviations, DS: Disposition, SV: Subject Visits</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>Form Name: Demographics</t>
-        </is>
-      </c>
+      <c r="A9" s="5" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Form Code: DM</t>
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>주의</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Repeat: FALSE</t>
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>- 'SAE'는 SDTM에서 보통 AE 도메인 내 Seriousness 변수로 표현합니다. 그래서 샘플은 SAE도 AE 코드로 표기했습니다.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>- 회사/프로젝트 표준에 따라 Form Name은 자유롭게 바꾸셔도 됩니다(코드는 SDTM에 맞추는 것을 권장).</t>
         </is>
       </c>
     </row>

</xml_diff>